<commit_message>
Integrated Long and Lat, installed folium
</commit_message>
<xml_diff>
--- a/clarkEase/pages/management/BuildingData.xlsx
+++ b/clarkEase/pages/management/BuildingData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\OneDrive - Clark University\Documents\GitHub\2023-Hackathon--ClarkEase\clarkEase\pages\management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D51208-D830-4BFE-A65A-1948C52DC987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A442E0B1-7AA2-4740-AC03-949D4B513DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{D82F770A-BD3E-4767-9656-DFBB943A2F32}"/>
   </bookViews>
@@ -423,8 +423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB90D1D7-0598-43F3-8C22-508072D7BA43}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -485,10 +485,10 @@
         <v>3</v>
       </c>
       <c r="G2">
-        <v>42.150709999999997</v>
+        <v>42.252001</v>
       </c>
       <c r="H2">
-        <v>71.491590000000002</v>
+        <v>-71.821079999999995</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -509,6 +509,12 @@
       </c>
       <c r="F3">
         <v>1</v>
+      </c>
+      <c r="G3">
+        <v>42.250010000000003</v>
+      </c>
+      <c r="H3">
+        <v>-71.826244000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added map marker functionality
</commit_message>
<xml_diff>
--- a/clarkEase/pages/management/BuildingData.xlsx
+++ b/clarkEase/pages/management/BuildingData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\OneDrive - Clark University\Documents\GitHub\2023-Hackathon--ClarkEase\clarkEase\pages\management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A442E0B1-7AA2-4740-AC03-949D4B513DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757CB748-88D6-43C8-A90E-B3254D15A45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{D82F770A-BD3E-4767-9656-DFBB943A2F32}"/>
   </bookViews>
@@ -59,9 +59,6 @@
     <t>MACD</t>
   </si>
   <si>
-    <t>True</t>
-  </si>
-  <si>
     <t>Blackstone Hall</t>
   </si>
   <si>
@@ -69,6 +66,9 @@
   </si>
   <si>
     <t>Longitude (E W)</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -424,7 +424,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,10 +459,10 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
         <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -470,13 +470,13 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -493,16 +493,16 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>4</v>

</xml_diff>

<commit_message>
Fill in building data
that took so long.
Added all of the data for every building on campus including coordinates
I hate google earth so much.
</commit_message>
<xml_diff>
--- a/clarkEase/pages/management/BuildingData.xlsx
+++ b/clarkEase/pages/management/BuildingData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\OneDrive - Clark University\Documents\GitHub\2023-Hackathon--ClarkEase\clarkEase\pages\management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757CB748-88D6-43C8-A90E-B3254D15A45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B85998-7435-449F-AC9B-321F671B1DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{D82F770A-BD3E-4767-9656-DFBB943A2F32}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{D82F770A-BD3E-4767-9656-DFBB943A2F32}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="56">
   <si>
     <t>Building Name</t>
   </si>
@@ -69,6 +69,141 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Maywood Street Apartments</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Admissions House</t>
+  </si>
+  <si>
+    <t>Admissions Center</t>
+  </si>
+  <si>
+    <t>BP</t>
+  </si>
+  <si>
+    <t>Bio-Lasry</t>
+  </si>
+  <si>
+    <t>Maywood Hall</t>
+  </si>
+  <si>
+    <t>Dana Commons</t>
+  </si>
+  <si>
+    <t>Dana Hall</t>
+  </si>
+  <si>
+    <t>Hughes Hall</t>
+  </si>
+  <si>
+    <t>Carlson Hall</t>
+  </si>
+  <si>
+    <t>University Center</t>
+  </si>
+  <si>
+    <t>ASEC</t>
+  </si>
+  <si>
+    <t>Geography Building</t>
+  </si>
+  <si>
+    <t>Jefferson Building</t>
+  </si>
+  <si>
+    <t>Atwood Hall</t>
+  </si>
+  <si>
+    <t>150 - 153 Woodland</t>
+  </si>
+  <si>
+    <t>Strassler Center</t>
+  </si>
+  <si>
+    <t>IDCE House</t>
+  </si>
+  <si>
+    <t>Anderson House</t>
+  </si>
+  <si>
+    <t>Carriage House</t>
+  </si>
+  <si>
+    <t>Beck House</t>
+  </si>
+  <si>
+    <t>CPG</t>
+  </si>
+  <si>
+    <t>Woodland RLH Houses</t>
+  </si>
+  <si>
+    <t>Clark Labs</t>
+  </si>
+  <si>
+    <t>Jonas Clark</t>
+  </si>
+  <si>
+    <t>Tilton</t>
+  </si>
+  <si>
+    <t>Higgins Café</t>
+  </si>
+  <si>
+    <t>Goddard Library</t>
+  </si>
+  <si>
+    <t>Bullock Hall</t>
+  </si>
+  <si>
+    <t>Wright Hall</t>
+  </si>
+  <si>
+    <t>Kneller Athletic Center</t>
+  </si>
+  <si>
+    <t>Dodd Hall</t>
+  </si>
+  <si>
+    <t>JSC Hall</t>
+  </si>
+  <si>
+    <t>Little Center</t>
+  </si>
+  <si>
+    <t>Gates House</t>
+  </si>
+  <si>
+    <t>Health Services</t>
+  </si>
+  <si>
+    <t>Estabrook Hall</t>
+  </si>
+  <si>
+    <t>Dolan Field House</t>
+  </si>
+  <si>
+    <t>Sackler Science Building</t>
+  </si>
+  <si>
+    <t>Traina Center</t>
+  </si>
+  <si>
+    <t>Corner House</t>
+  </si>
+  <si>
+    <t>Alumni Affairs</t>
+  </si>
+  <si>
+    <t>Yes (Through Geography Building)</t>
   </si>
 </sst>
 </file>
@@ -421,10 +556,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB90D1D7-0598-43F3-8C22-508072D7BA43}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -435,8 +571,8 @@
     <col min="4" max="4" width="23.77734375" customWidth="1"/>
     <col min="5" max="5" width="20.21875" customWidth="1"/>
     <col min="6" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="50.88671875" customWidth="1"/>
-    <col min="8" max="8" width="58.109375" customWidth="1"/>
+    <col min="7" max="7" width="20.88671875" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -485,10 +621,10 @@
         <v>3</v>
       </c>
       <c r="G2">
-        <v>42.252001</v>
+        <v>42.251904699999997</v>
       </c>
       <c r="H2">
-        <v>-71.821079999999995</v>
+        <v>-71.821193199999996</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -508,16 +644,1109 @@
         <v>4</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3">
-        <v>42.250010000000003</v>
+        <v>42.249926600000002</v>
       </c>
       <c r="H3">
-        <v>-71.826244000000003</v>
+        <v>-71.826223200000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>42.249732399999999</v>
+      </c>
+      <c r="H4">
+        <v>-71.824758200000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>42.250225899999997</v>
+      </c>
+      <c r="H5">
+        <v>-71.825493300000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>42.249605799999998</v>
+      </c>
+      <c r="H6">
+        <v>-71.824285700000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>42.249559599999998</v>
+      </c>
+      <c r="H7">
+        <v>-71.824318399999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>42.2506464150174</v>
+      </c>
+      <c r="H8">
+        <v>-71.823706839973397</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>42.250460211016502</v>
+      </c>
+      <c r="H9">
+        <v>-71.824292284852206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>42.250863000000003</v>
+      </c>
+      <c r="H10">
+        <v>-71.824881000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>42.251194296861897</v>
+      </c>
+      <c r="H11">
+        <v>-71.825369231908198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>42.251631000000003</v>
+      </c>
+      <c r="H12">
+        <v>-71.825288999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>42.2517599693455</v>
+      </c>
+      <c r="H13">
+        <v>-71.824678493857405</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>42.251025900000002</v>
+      </c>
+      <c r="H14">
+        <v>-71.825915100000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>42.249903444625801</v>
+      </c>
+      <c r="H15">
+        <v>-71.823514825395804</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>42.2501465</v>
+      </c>
+      <c r="H16">
+        <v>-71.823159700000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>42.250216700000003</v>
+      </c>
+      <c r="H17">
+        <v>-71.822130799999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>42.250632899999999</v>
+      </c>
+      <c r="H18">
+        <v>-71.822094699999994</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>42.250836200000002</v>
+      </c>
+      <c r="H19">
+        <v>-71.821846600000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>42.251299199999998</v>
+      </c>
+      <c r="H20">
+        <v>-71.822243</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>42.251707799999998</v>
+      </c>
+      <c r="H21">
+        <v>-71.822080099999994</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>42.252237000000001</v>
+      </c>
+      <c r="H22">
+        <v>-71.821273000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>42.251729099999999</v>
+      </c>
+      <c r="H23">
+        <v>-71.820751000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>42.252571000000003</v>
+      </c>
+      <c r="H24">
+        <v>-71.8214629</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>42.252694499999997</v>
+      </c>
+      <c r="H25">
+        <v>-71.820688799999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>42.253386800000001</v>
+      </c>
+      <c r="H26">
+        <v>-71.820839000000007</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>42.253386800000001</v>
+      </c>
+      <c r="H27">
+        <v>-71.820839000000007</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>42.251486</v>
+      </c>
+      <c r="H28">
+        <v>-71.820943999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>42.251382599999999</v>
+      </c>
+      <c r="H29">
+        <v>-71.820092700000004</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>42.251008004116798</v>
+      </c>
+      <c r="H30">
+        <v>-71.823101468429101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>42.250132299999997</v>
+      </c>
+      <c r="H31">
+        <v>-71.823175699999993</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32">
+        <v>4</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <v>42.251748900000003</v>
+      </c>
+      <c r="H32">
+        <v>-71.823528199999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>42.251337372301698</v>
+      </c>
+      <c r="H33">
+        <v>-71.823943865868799</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>42.2519852</v>
+      </c>
+      <c r="H34">
+        <v>-71.8230693</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>42.252198</v>
+      </c>
+      <c r="H35">
+        <v>-71.824418100000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>42.252743844993198</v>
+      </c>
+      <c r="H36">
+        <v>-71.823323494843706</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+      <c r="F37">
+        <v>3</v>
+      </c>
+      <c r="G37">
+        <v>42.253313804552803</v>
+      </c>
+      <c r="H37">
+        <v>-71.823097797768995</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>42.252621712263199</v>
+      </c>
+      <c r="H38">
+        <v>-71.822648302412404</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>42.253440148866602</v>
+      </c>
+      <c r="H39">
+        <v>-71.822570541270096</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>42.252871800000001</v>
+      </c>
+      <c r="H40">
+        <v>-71.827541600000004</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>42.2521792</v>
+      </c>
+      <c r="H41">
+        <v>-71.822451599999994</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="G42">
+        <v>42.249255699999999</v>
+      </c>
+      <c r="H42">
+        <v>-71.830059899999995</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>42.253954999999998</v>
+      </c>
+      <c r="H43">
+        <v>-71.824838</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>42.252325499999998</v>
+      </c>
+      <c r="H44">
+        <v>-71.821945999999997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>42.252980600000001</v>
+      </c>
+      <c r="H45">
+        <v>-71.821111000000002</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>